<commit_message>
Added E00019,E00020, added a gitignore for temp when editing .xlsx
</commit_message>
<xml_diff>
--- a/Index SONIA 1/INDEX_SONIA_1.xlsx
+++ b/Index SONIA 1/INDEX_SONIA_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sonia\hardware_index_sonia1\Index SONIA 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\School_or_internship_BAC\SONIA\hardware_index_sonia1\Index SONIA 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A05914A5-6D81-4B74-8CE1-0A73DE060249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC201050-7AF6-4802-ACFC-DF11D04F4C14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21600" yWindow="990" windowWidth="28560" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LISTE" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="206">
   <si>
     <t>Catégorie</t>
   </si>
@@ -640,6 +640,21 @@
   </si>
   <si>
     <t>Index SONIA 1\E00019</t>
+  </si>
+  <si>
+    <t>E00020</t>
+  </si>
+  <si>
+    <t>RES 0.001 OHM 1% 3W 2512</t>
+  </si>
+  <si>
+    <t>1 mOhms ±1% 3W Chip Resistor 2512 (6432 Metric) Automotive AEC-Q200, Current Sense, Moisture Resistant Metal Element</t>
+  </si>
+  <si>
+    <t>Index SONIA 1\E00020</t>
+  </si>
+  <si>
+    <t>CRE2512-FZ-R001E-3</t>
   </si>
 </sst>
 </file>
@@ -783,7 +798,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -889,6 +904,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1632,8 +1650,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E488228-7BB2-48E8-8D64-0FE9665C033D}" name="Tableau13" displayName="Tableau13" ref="A5:N24" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A5:N24" xr:uid="{58943F4C-4DE4-4629-A635-9F2408F28BF2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6E488228-7BB2-48E8-8D64-0FE9665C033D}" name="Tableau13" displayName="Tableau13" ref="A5:N26" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A5:N26" xr:uid="{58943F4C-4DE4-4629-A635-9F2408F28BF2}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{CC1476A6-385C-4BE9-9D3F-2770D445CE3D}" name="Numéro" dataDxfId="27" totalsRowDxfId="26"/>
     <tableColumn id="2" xr3:uid="{819093A4-4C18-4D06-9052-08A813483FA7}" name="Catégorie" dataDxfId="25" totalsRowDxfId="24"/>
@@ -1941,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2778,10 +2796,10 @@
       <c r="N23" s="24"/>
     </row>
     <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="20" t="s">
         <v>194</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="21" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="21" t="s">
@@ -2790,32 +2808,88 @@
       <c r="D24" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="21" t="s">
         <v>197</v>
       </c>
-      <c r="G24" s="35" t="s">
+      <c r="G24" s="21" t="s">
         <v>198</v>
       </c>
       <c r="H24" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="I24" s="35" t="s">
+      <c r="I24" s="21" t="s">
         <v>62</v>
       </c>
       <c r="J24" s="23"/>
       <c r="K24" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="L24" s="35" t="s">
+      <c r="L24" s="21" t="s">
         <v>66</v>
       </c>
       <c r="M24" s="24" t="s">
         <v>199</v>
       </c>
       <c r="N24" s="24"/>
+    </row>
+    <row r="25" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>202</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="J25" s="23"/>
+      <c r="K25" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="L25" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="M25" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="N25" s="24"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -2836,14 +2910,15 @@
     <hyperlink ref="H22" r:id="rId14" xr:uid="{D649E74A-843A-4C20-A7A1-A529E97992EA}"/>
     <hyperlink ref="H23" r:id="rId15" xr:uid="{D2F0A9A1-D0FD-4E67-ADC8-835F7E0B60B7}"/>
     <hyperlink ref="H24" r:id="rId16" display="Index SONIA 1\E00018" xr:uid="{42EE1618-EC14-43C7-A722-D6B03216A17D}"/>
+    <hyperlink ref="H25" r:id="rId17" xr:uid="{24628E5F-4EFD-4084-8B48-06C5FA7C4DF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
   <ignoredErrors>
     <ignoredError sqref="D6" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="1">
-    <tablePart r:id="rId18"/>
+    <tablePart r:id="rId19"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>